<commit_message>
feat: add/update test cases for MyInfo, Time, Recruitment, PIM, Leave
</commit_message>
<xml_diff>
--- a/manual-test/Recruitment Test Case - OrangeHRM.xlsx
+++ b/manual-test/Recruitment Test Case - OrangeHRM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="141">
   <si>
     <t>Postive Test Case</t>
   </si>
@@ -227,18 +227,6 @@
     <t>TC_RC_013</t>
   </si>
   <si>
-    <t>Klik tombol Edit (ikon pensil)</t>
-  </si>
-  <si>
-    <t>1. Klik tombol Edit di baris kandidat</t>
-  </si>
-  <si>
-    <t>Dialihkan ke halaman edit kandidat</t>
-  </si>
-  <si>
-    <t>TC_RC_014</t>
-  </si>
-  <si>
     <t>Klik tombol Delete (ikon tempat sampah)</t>
   </si>
   <si>
@@ -249,19 +237,19 @@
     <t>Kandidat terhapus setelah konfirmasi</t>
   </si>
   <si>
+    <t>TC_RC_014</t>
+  </si>
+  <si>
+    <t>Klik tombol Download Resume (ikon panah bawah)</t>
+  </si>
+  <si>
+    <t>1. Klik Download di baris kandidat</t>
+  </si>
+  <si>
+    <t>File resume terunduh</t>
+  </si>
+  <si>
     <t>TC_RC_015</t>
-  </si>
-  <si>
-    <t>Klik tombol Download Resume (ikon panah bawah)</t>
-  </si>
-  <si>
-    <t>1. Klik Download di baris kandidat</t>
-  </si>
-  <si>
-    <t>File resume terunduh</t>
-  </si>
-  <si>
-    <t>TC_RC_016</t>
   </si>
   <si>
     <t>Semua filter digunakan sekaligus</t>
@@ -277,31 +265,31 @@
     <t>Data yang muncul cocok dengan semua kriteria</t>
   </si>
   <si>
+    <t>TC_RC_016</t>
+  </si>
+  <si>
+    <t>Urutkan tabel berdasarkan kolom tertentu</t>
+  </si>
+  <si>
+    <t>1. Klik kolom Vacancy atau Date of Application</t>
+  </si>
+  <si>
+    <t>Data diurutkan sesuai kolom</t>
+  </si>
+  <si>
     <t>TC_RC_017</t>
   </si>
   <si>
-    <t>Urutkan tabel berdasarkan kolom tertentu</t>
-  </si>
-  <si>
-    <t>1. Klik kolom Vacancy atau Date of Application</t>
-  </si>
-  <si>
-    <t>Data diurutkan sesuai kolom</t>
+    <t>Hover ke ikon-ikon Action</t>
+  </si>
+  <si>
+    <t>1. Arahkan kursor ke ikon View, Edit, Delete, Download</t>
+  </si>
+  <si>
+    <t>Tooltip nama aksi muncul sesuai ikon</t>
   </si>
   <si>
     <t>TC_RC_018</t>
-  </si>
-  <si>
-    <t>Hover ke ikon-ikon Action</t>
-  </si>
-  <si>
-    <t>1. Arahkan kursor ke ikon View, Edit, Delete, Download</t>
-  </si>
-  <si>
-    <t>Tooltip nama aksi muncul sesuai ikon</t>
-  </si>
-  <si>
-    <t>TC_RC_019</t>
   </si>
   <si>
     <t>Navigasi ke tab Vacancies</t>
@@ -1117,10 +1105,10 @@
         <v>77</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>13</v>
@@ -1131,16 +1119,16 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>83</v>
@@ -1198,32 +1186,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26">
@@ -1251,22 +1216,22 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>14</v>
@@ -1275,22 +1240,22 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="F28" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>14</v>
@@ -1298,22 +1263,22 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>112</v>
-      </c>
       <c r="F29" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>14</v>
@@ -1321,22 +1286,22 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="F30" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>14</v>
@@ -1344,22 +1309,22 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>14</v>
@@ -1367,22 +1332,22 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="F32" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>14</v>
@@ -1390,22 +1355,22 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>14</v>
@@ -1413,22 +1378,22 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>14</v>
@@ -1436,22 +1401,22 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="F35" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>14</v>
@@ -1459,22 +1424,22 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>14</v>

</xml_diff>